<commit_message>
Add Daftar Hadir & Nilai
</commit_message>
<xml_diff>
--- a/resources/format_soal.xlsx
+++ b/resources/format_soal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\web\ujian_akm\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959D9D0A-6D23-4DBF-986E-5FD0F636F65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034E1FBE-CDC0-4699-A298-637863428A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,18 +41,8 @@
     <author>asd412id</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{830BAEB4-1FB4-4909-B3A4-6DD8B8C2915E}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8ADDDF23-76EF-4B24-9C6F-8CBEEB0CDFA0}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Cara Pengisian:</t>
-        </r>
         <r>
           <rPr>
             <sz val="9"/>
@@ -60,14 +50,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-Masukkan teks pernyataan untuk jenis soal Benar/Salah dan Menjodohkan.
+          <t>Masukkan teks pernyataan untuk jenis soal Benar/Salah dan Menjodohkan.
 Untuk jenis soal Benar/Salah, maka cukup mengisi label dengan alias dari pernyataan
 Untuk jenis soal Menjodohkan, pisahkan label antara opsi yang ingin dijodohkan dan opsi yang dijodohkan dengan tanda koma (,)</t>
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{886D5BD8-AA02-4060-924A-034A9289F643}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{81598768-220D-46B2-BF21-5D43A5881349}">
       <text>
         <r>
           <rPr>
@@ -81,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{D13B3E9A-56C9-4E25-AAF5-CF3E7481DD34}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{986C9B14-D2E3-42E4-903F-5BB16F3B4E08}">
       <text>
         <r>
           <rPr>
@@ -505,7 +494,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,13 +518,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -723,6 +705,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -731,18 +725,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,35 +1023,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="K3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="K3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1357,28 +1339,28 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="18" t="s">
+      <c r="L7" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="N7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="O7" s="16" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweak excel import: image position more flexible
</commit_message>
<xml_diff>
--- a/resources/format_soal.xlsx
+++ b/resources/format_soal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\web\ujian_akm\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB955D7-5DF6-4405-94DE-3129FA00A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D5A65-C259-4EAD-ACCC-E56240285518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>No.</t>
   </si>
@@ -372,7 +372,26 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Untuk memasukkan gambar:
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Untuk memasukkan gambar:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Copy/Insert gambar ke tepat ke dalam cell (semua bagian gambar di resize agar berada di dalam cell)
 </t>
     </r>
@@ -408,17 +427,39 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Rata Tengah:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Pastikan sisi kiri-kanan gambar tidak menyentuh sisi kiri-kanan cell
+      <t xml:space="preserve">Standar: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Letak gambar pada cell agak ke kiri tetapi tidak menyentuh sisi kiri cell</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Rata Tengah:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Letak gambar berada di tengah-tengah cell secara proporsional, atau sisi kiri-kanan gambar menyentuh sisi kiri-kanan cell
 </t>
     </r>
     <r>
@@ -485,6 +526,51 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Sisi bawah gambar menyentuh sisi bawah cell
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Menyisipkan gambar di antara kalimat:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Buat space antar kalimat dengan menekan </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">alt+enter </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2(dua) kali sehingga terdapat baris kosong di antara kalimat. Kemudian masukkan gambar ke dalam cell tersebut dengan memperhatikan posisi gambar
 ATAU
 Gunakan kode gambar:
 </t>
@@ -601,13 +687,16 @@
       </rPr>
       <t>pada contoh di atas adalah ekstensi gambar yang diupload di menu Media. Jika gambar yang Anda upload berekstensi lain (png, jpeg) maka sesuaikan pada kode gambar</t>
     </r>
+  </si>
+  <si>
+    <t>Buka Sheet "Soal" untuk mulai memasukkan soal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,8 +757,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +860,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -782,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -833,10 +951,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -847,6 +968,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9966FF"/>
       <color rgb="FF00CC99"/>
     </mruColors>
   </colors>
@@ -1127,12 +1249,12 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1143,6 +1265,9 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
+      <c r="I1" s="20" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">

</xml_diff>

<commit_message>
Auto-delete soal image's folder when deleting soal
</commit_message>
<xml_diff>
--- a/resources/format_soal.xlsx
+++ b/resources/format_soal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\web\ujian_akm\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5D5A65-C259-4EAD-ACCC-E56240285518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CC517A-DC91-497A-B1B2-3AF8A8814700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,6 +41,35 @@
     <author>asd412id</author>
   </authors>
   <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8FB3E133-4286-45D4-BF85-8803B6767972}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Pilih Jenis Soal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PG = Pilihan Ganda
+PGK = Pilihan Ganda Kompleks
+IS = Isian Singkat
+U = Uraian
+BS = Benar/Salah
+JD = Menjodohkan</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8ADDDF23-76EF-4B24-9C6F-8CBEEB0CDFA0}">
       <text>
         <r>
@@ -696,7 +725,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -773,6 +802,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -948,17 +990,17 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1258,29 +1300,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="I1" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="145.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
       <c r="K3" s="19" t="s">
         <v>33</v>
       </c>
@@ -1292,235 +1334,235 @@
       <c r="Q3" s="19"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:17" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>